<commit_message>
new example with real inp file included
</commit_message>
<xml_diff>
--- a/example/example_mapping.xlsx
+++ b/example/example_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\CS570 (1)\FEA_schema_template\test folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Claire\FEA_schema_template\nm_curation_batch_template_generation\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3526CB7-AE62-4F1F-AC57-55B3BAAC1B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D703113F-EBCD-414A-8B83-BE90E51A43B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18120" yWindow="192" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="-200" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -426,17 +426,19 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="14.1015625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.47265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.06640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.53125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.46484375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -462,7 +464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -470,13 +472,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -488,7 +490,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -496,10 +498,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E3">
         <v>0.8</v>
@@ -514,7 +516,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -522,10 +524,10 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E4">
         <v>0.8</v>
@@ -540,7 +542,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -548,13 +550,13 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>23</v>

</xml_diff>